<commit_message>
Round execution times of 0.015 and 0.016 down to 0.
</commit_message>
<xml_diff>
--- a/perf.xlsx
+++ b/perf.xlsx
@@ -3639,7 +3639,7 @@
         <v>11.372727272727273</v>
       </c>
       <c r="C112" s="3">
-        <f t="shared" ref="C112:H112" si="0">AVERAGE(C2:C111)</f>
+        <f t="shared" ref="C112:G112" si="0">AVERAGE(C2:C111)</f>
         <v>20683.027272727271</v>
       </c>
       <c r="D112" s="3">
@@ -3672,7 +3672,7 @@
         <v>11</v>
       </c>
       <c r="C113" s="3">
-        <f t="shared" ref="C113:H113" si="2">MEDIAN(C2:C111)</f>
+        <f t="shared" ref="C113:G113" si="2">MEDIAN(C2:C111)</f>
         <v>100</v>
       </c>
       <c r="D113" s="3">
@@ -3759,7 +3759,7 @@
         <v>121.60899999999999</v>
       </c>
       <c r="D2">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>642.96900000000005</v>
@@ -3840,13 +3840,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0.14099999999999999</v>
@@ -3944,7 +3944,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -4016,7 +4016,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -4025,10 +4025,10 @@
         <v>3.1E-2</v>
       </c>
       <c r="F12">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0.96799999999999997</v>
@@ -4042,7 +4042,7 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4068,13 +4068,13 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -4126,13 +4126,13 @@
         <v>3.1E-2</v>
       </c>
       <c r="E16">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>2.984</v>
@@ -4146,7 +4146,7 @@
         <v>12</v>
       </c>
       <c r="C17">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>3.1E-2</v>
@@ -4181,7 +4181,7 @@
         <v>0.109</v>
       </c>
       <c r="F18">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>3.1E-2</v>
@@ -4276,7 +4276,7 @@
         <v>11</v>
       </c>
       <c r="C22">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4314,7 +4314,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="G23">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0.20300000000000001</v>
@@ -4331,7 +4331,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4340,7 +4340,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>6.3E-2</v>
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4383,7 +4383,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4473,7 +4473,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4493,7 +4493,7 @@
         <v>0.65600000000000003</v>
       </c>
       <c r="F30">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <v>9.2999999999999999E-2</v>
@@ -4629,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -4640,7 +4640,7 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4698,7 +4698,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="E38">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -4828,7 +4828,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="E43">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -4877,7 +4877,7 @@
         <v>0.71899999999999997</v>
       </c>
       <c r="D45">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>7.0629999999999997</v>
@@ -4912,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -4932,7 +4932,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -4952,16 +4952,16 @@
         <v>15</v>
       </c>
       <c r="C48">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>9.4E-2</v>
       </c>
       <c r="E48">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <v>3.1E-2</v>
@@ -5033,13 +5033,13 @@
         <v>4.7E-2</v>
       </c>
       <c r="D51">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E51">
         <v>0.46899999999999997</v>
       </c>
       <c r="F51">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G51">
         <v>3.1E-2</v>
@@ -5059,7 +5059,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="D52">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E52">
         <v>1.016</v>
@@ -5082,13 +5082,13 @@
         <v>11</v>
       </c>
       <c r="C53">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F53">
         <v>4.7E-2</v>
@@ -5108,7 +5108,7 @@
         <v>13</v>
       </c>
       <c r="C54">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D54">
         <v>3.2000000000000001E-2</v>
@@ -5117,7 +5117,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="F54">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <v>4.7E-2</v>
@@ -5160,13 +5160,13 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -5195,7 +5195,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G57">
         <v>3.2000000000000001E-2</v>
@@ -5212,7 +5212,7 @@
         <v>19</v>
       </c>
       <c r="C58">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D58">
         <v>0.375</v>
@@ -5224,7 +5224,7 @@
         <v>0.26600000000000001</v>
       </c>
       <c r="G58">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H58">
         <v>239.28100000000001</v>
@@ -5241,13 +5241,13 @@
         <v>4.7E-2</v>
       </c>
       <c r="D59">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -5267,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>3.1E-2</v>
@@ -5383,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -5420,7 +5420,7 @@
         <v>20</v>
       </c>
       <c r="C66">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D66">
         <v>0.375</v>
@@ -5446,7 +5446,7 @@
         <v>14</v>
       </c>
       <c r="C67">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <v>0.14099999999999999</v>
@@ -5455,10 +5455,10 @@
         <v>0.219</v>
       </c>
       <c r="F67">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H67">
         <v>4.1879999999999997</v>
@@ -5472,7 +5472,7 @@
         <v>14</v>
       </c>
       <c r="C68">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D68">
         <v>6.2E-2</v>
@@ -5481,7 +5481,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="F68">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <v>3.1E-2</v>
@@ -5501,7 +5501,7 @@
         <v>0.156</v>
       </c>
       <c r="D69">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0.109</v>
@@ -5591,7 +5591,7 @@
         <v>0</v>
       </c>
       <c r="H72">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -5611,7 +5611,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="F73">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G73">
         <v>3.1E-2</v>
@@ -5634,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -5643,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="H74">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -5822,7 +5822,7 @@
         <v>0.90600000000000003</v>
       </c>
       <c r="G81">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H81">
         <v>62.545999999999999</v>
@@ -5868,10 +5868,10 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -5888,7 +5888,7 @@
         <v>17</v>
       </c>
       <c r="C84">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D84">
         <v>6.2E-2</v>
@@ -5946,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="E86">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -5955,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -5969,7 +5969,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="D87">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E87">
         <v>3.468</v>
@@ -6024,10 +6024,10 @@
         <v>4.7E-2</v>
       </c>
       <c r="E89">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -6070,10 +6070,10 @@
         <v>18</v>
       </c>
       <c r="C91">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>0.109</v>
@@ -6125,7 +6125,7 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E93">
         <v>0.156</v>
@@ -6151,13 +6151,13 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -6235,13 +6235,13 @@
         <v>0</v>
       </c>
       <c r="F97">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G97">
         <v>0</v>
       </c>
       <c r="H97">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -6258,7 +6258,7 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -6290,7 +6290,7 @@
         <v>0.156</v>
       </c>
       <c r="G99">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="H99">
         <v>26.125</v>
@@ -6304,16 +6304,16 @@
         <v>11</v>
       </c>
       <c r="C100">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="D100">
         <v>0</v>
       </c>
       <c r="E100">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -6342,7 +6342,7 @@
         <v>0.219</v>
       </c>
       <c r="G101">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H101">
         <v>10.125999999999999</v>
@@ -6385,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="D103">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -6397,7 +6397,7 @@
         <v>0</v>
       </c>
       <c r="H103">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -6414,7 +6414,7 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -6538,19 +6538,19 @@
         <v>17</v>
       </c>
       <c r="C109">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D109">
         <v>0.125</v>
       </c>
       <c r="E109">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F109">
         <v>0</v>
       </c>
       <c r="G109">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="H109">
         <v>29.422999999999998</v>
@@ -6564,7 +6564,7 @@
         <v>7</v>
       </c>
       <c r="C110">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -6573,13 +6573,13 @@
         <v>0</v>
       </c>
       <c r="F110">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="G110">
         <v>0</v>
       </c>
       <c r="H110">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -6617,28 +6617,28 @@
         <v>11.372727272727273</v>
       </c>
       <c r="C112" s="4">
-        <f t="shared" ref="C112:H112" si="0">AVERAGE(C2:C111)</f>
-        <v>1.3154636363636347</v>
+        <f t="shared" ref="C112:G112" si="0">AVERAGE(C2:C111)</f>
+        <v>1.3127727272727276</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="0"/>
-        <v>0.18041818181818184</v>
+        <v>0.17830909090909094</v>
       </c>
       <c r="E112" s="4">
         <f t="shared" si="0"/>
-        <v>6.4781818181818149</v>
+        <v>6.4754545454545482</v>
       </c>
       <c r="F112" s="4">
         <f t="shared" si="0"/>
-        <v>0.34189999999999987</v>
+        <v>0.33938181818181812</v>
       </c>
       <c r="G112" s="4">
         <f t="shared" si="0"/>
-        <v>0.18806363636363646</v>
+        <v>0.18638181818181826</v>
       </c>
       <c r="H112" s="4">
         <f t="shared" ref="H112" si="1">AVERAGE(H2:H111)</f>
-        <v>56.729715596330266</v>
+        <v>56.72830275229358</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -6650,16 +6650,16 @@
         <v>11</v>
       </c>
       <c r="C113" s="4">
-        <f t="shared" ref="C113:H113" si="2">MEDIAN(C2:C111)</f>
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" ref="C113:G113" si="2">MEDIAN(C2:C111)</f>
+        <v>0</v>
       </c>
       <c r="D113" s="4">
         <f t="shared" si="2"/>
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E113" s="4">
         <f t="shared" si="2"/>
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="F113" s="4">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Roun anomalous times below 0.01s to 0.
</commit_message>
<xml_diff>
--- a/perf.xlsx
+++ b/perf.xlsx
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -4120,10 +4120,10 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4149,10 +4149,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -4172,13 +4172,13 @@
         <v>14</v>
       </c>
       <c r="C18">
-        <v>6.3E-2</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -4224,7 +4224,7 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>6.2E-2</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>1.5469999999999999</v>
@@ -4282,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -4302,16 +4302,16 @@
         <v>11</v>
       </c>
       <c r="C23">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -4395,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4432,19 +4432,19 @@
         <v>17</v>
       </c>
       <c r="C28">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0.375</v>
       </c>
       <c r="E28">
-        <v>0.17199999999999999</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0.20399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>36.265999999999998</v>
@@ -4484,7 +4484,7 @@
         <v>19</v>
       </c>
       <c r="C30">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0.20300000000000001</v>
@@ -4588,7 +4588,7 @@
         <v>14</v>
       </c>
       <c r="C34">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -4597,7 +4597,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -4692,10 +4692,10 @@
         <v>13</v>
       </c>
       <c r="C38">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -4704,7 +4704,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <v>2.5470000000000002</v>
@@ -4825,7 +4825,7 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -4941,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4964,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <v>11.266</v>
@@ -4978,7 +4978,7 @@
         <v>19</v>
       </c>
       <c r="C49">
-        <v>6.3E-2</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>0.29699999999999999</v>
@@ -5030,7 +5030,7 @@
         <v>14</v>
       </c>
       <c r="C51">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -5042,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <v>6.0940000000000003</v>
@@ -5068,7 +5068,7 @@
         <v>0.40600000000000003</v>
       </c>
       <c r="G52">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <v>521.11</v>
@@ -5091,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="G53">
         <v>4.7E-2</v>
@@ -5111,10 +5111,10 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -5186,7 +5186,7 @@
         <v>14</v>
       </c>
       <c r="C57">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D57">
         <v>6.3E-2</v>
@@ -5198,7 +5198,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="H57">
         <v>0.81200000000000006</v>
@@ -5218,7 +5218,7 @@
         <v>0.375</v>
       </c>
       <c r="E58">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0.26600000000000001</v>
@@ -5238,7 +5238,7 @@
         <v>10</v>
       </c>
       <c r="C59">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -5270,13 +5270,13 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="H60">
         <v>1.1719999999999999</v>
@@ -5290,7 +5290,7 @@
         <v>17</v>
       </c>
       <c r="C61">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0.96899999999999997</v>
@@ -5348,7 +5348,7 @@
         <v>0.76500000000000001</v>
       </c>
       <c r="E63">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0.29699999999999999</v>
@@ -5478,13 +5478,13 @@
         <v>6.2E-2</v>
       </c>
       <c r="E68">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="F68">
         <v>0</v>
       </c>
       <c r="G68">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="H68">
         <v>2.5150000000000001</v>
@@ -5504,7 +5504,7 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="F69">
         <v>0.109</v>
@@ -5602,19 +5602,19 @@
         <v>12</v>
       </c>
       <c r="C73">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="D73">
         <v>6.3E-2</v>
       </c>
       <c r="E73">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>0.218</v>
@@ -5680,16 +5680,16 @@
         <v>16</v>
       </c>
       <c r="C76">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>1.5</v>
       </c>
       <c r="F76">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="G76">
         <v>4.7E-2</v>
@@ -5966,7 +5966,7 @@
         <v>20</v>
       </c>
       <c r="C87">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -6047,7 +6047,7 @@
         <v>0.81200000000000006</v>
       </c>
       <c r="D90">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="E90">
         <v>0.51500000000000001</v>
@@ -6076,10 +6076,10 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>3.2000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G91">
         <v>9.4E-2</v>
@@ -6209,7 +6209,7 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="F96">
-        <v>4.7E-2</v>
+        <v>0</v>
       </c>
       <c r="G96">
         <v>0.67200000000000004</v>
@@ -6278,7 +6278,7 @@
         <v>17</v>
       </c>
       <c r="C99">
-        <v>6.3E-2</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <v>0.14099999999999999</v>
@@ -6330,7 +6330,7 @@
         <v>16</v>
       </c>
       <c r="C101">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="D101">
         <v>0.29699999999999999</v>
@@ -6356,7 +6356,7 @@
         <v>18</v>
       </c>
       <c r="C102">
-        <v>6.3E-2</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0.84399999999999997</v>
@@ -6618,27 +6618,27 @@
       </c>
       <c r="C112" s="4">
         <f t="shared" ref="C112:G112" si="0">AVERAGE(C2:C111)</f>
-        <v>1.3127727272727276</v>
+        <v>1.3052363636363638</v>
       </c>
       <c r="D112" s="4">
         <f t="shared" si="0"/>
-        <v>0.17830909090909094</v>
+        <v>0.17574545454545462</v>
       </c>
       <c r="E112" s="4">
         <f t="shared" si="0"/>
-        <v>6.4754545454545482</v>
+        <v>6.4680818181818216</v>
       </c>
       <c r="F112" s="4">
         <f t="shared" si="0"/>
-        <v>0.33938181818181812</v>
+        <v>0.33724545454545463</v>
       </c>
       <c r="G112" s="4">
         <f t="shared" si="0"/>
-        <v>0.18638181818181826</v>
+        <v>0.18225454545454547</v>
       </c>
       <c r="H112" s="4">
         <f t="shared" ref="H112" si="1">AVERAGE(H2:H111)</f>
-        <v>56.72830275229358</v>
+        <v>56.727587155963306</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Swapped aStar1 and aStarBase columns.
</commit_message>
<xml_diff>
--- a/perf.xlsx
+++ b/perf.xlsx
@@ -736,11 +736,11 @@
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -752,19 +752,19 @@
         <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>
@@ -3714,11 +3714,11 @@
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3730,19 +3730,19 @@
         <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>

</xml_diff>